<commit_message>
Updated ES3 HW matrix
</commit_message>
<xml_diff>
--- a/doc/OpenGL ES 3 Hardware Matrix.xlsx
+++ b/doc/OpenGL ES 3 Hardware Matrix.xlsx
@@ -1180,8 +1180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="U34" sqref="U34"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1705,8 +1705,8 @@
       <c r="C17" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>2</v>
+      <c r="D17" s="6" t="s">
+        <v>1</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>2</v>
@@ -12948,13 +12948,21 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="R147:S147"/>
-    <mergeCell ref="R154:S154"/>
-    <mergeCell ref="R12:S12"/>
-    <mergeCell ref="R56:S56"/>
-    <mergeCell ref="R85:S85"/>
-    <mergeCell ref="R95:S95"/>
-    <mergeCell ref="R105:S105"/>
+    <mergeCell ref="H105:J105"/>
+    <mergeCell ref="H147:J147"/>
+    <mergeCell ref="H154:J154"/>
+    <mergeCell ref="N154:P154"/>
+    <mergeCell ref="N105:P105"/>
+    <mergeCell ref="L154:M154"/>
+    <mergeCell ref="L147:M147"/>
+    <mergeCell ref="L105:M105"/>
+    <mergeCell ref="N147:P147"/>
+    <mergeCell ref="H95:J95"/>
+    <mergeCell ref="L95:M95"/>
+    <mergeCell ref="N95:P95"/>
+    <mergeCell ref="H56:J56"/>
+    <mergeCell ref="L56:M56"/>
+    <mergeCell ref="N56:P56"/>
     <mergeCell ref="A1:S1"/>
     <mergeCell ref="A2:S2"/>
     <mergeCell ref="A4:S4"/>
@@ -12971,21 +12979,13 @@
     <mergeCell ref="H85:J85"/>
     <mergeCell ref="L85:M85"/>
     <mergeCell ref="N85:P85"/>
-    <mergeCell ref="H95:J95"/>
-    <mergeCell ref="L95:M95"/>
-    <mergeCell ref="N95:P95"/>
-    <mergeCell ref="H56:J56"/>
-    <mergeCell ref="L56:M56"/>
-    <mergeCell ref="N56:P56"/>
-    <mergeCell ref="H105:J105"/>
-    <mergeCell ref="H147:J147"/>
-    <mergeCell ref="H154:J154"/>
-    <mergeCell ref="N154:P154"/>
-    <mergeCell ref="N105:P105"/>
-    <mergeCell ref="L154:M154"/>
-    <mergeCell ref="L147:M147"/>
-    <mergeCell ref="L105:M105"/>
-    <mergeCell ref="N147:P147"/>
+    <mergeCell ref="R147:S147"/>
+    <mergeCell ref="R154:S154"/>
+    <mergeCell ref="R12:S12"/>
+    <mergeCell ref="R56:S56"/>
+    <mergeCell ref="R85:S85"/>
+    <mergeCell ref="R95:S95"/>
+    <mergeCell ref="R105:S105"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A4" r:id="rId1" display="http://www.g-truc.net"/>

</xml_diff>